<commit_message>
feat: updates on rules
</commit_message>
<xml_diff>
--- a/containers/openltablets_server/brms/programming-grid/programming-grid-approval-rules.xlsx
+++ b/containers/openltablets_server/brms/programming-grid/programming-grid-approval-rules.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>SimpleRules Boolean programmingGridApprovalRule1 (Boolean fullWeek, Integer channelsPerDay, Integer weekUsedMinutes)</t>
   </si>
@@ -33,7 +33,10 @@
     <t>result</t>
   </si>
   <si>
-    <t>12 .. 72</t>
+    <t>5 .. 72</t>
+  </si>
+  <si>
+    <t>2100 .. 10080</t>
   </si>
 </sst>
 </file>
@@ -464,8 +467,8 @@
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10">
-        <v>10080.0</v>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="E4" s="11" t="b">
         <f>True</f>

</xml_diff>